<commit_message>
Kalender toegevoegd aan naslagwerk
Interactieve en filterbare kalender toegevoegd waarin de verschillende relevante perioden en momenten vermeld staan. Deze kalender is nu de landingspagina voor de kalendersectie. De overige onderdelen (grafiek en tabellen) zijn eveneens geüpdate naar collegejaar 2025.

Let op! De kalender wordt niet direct ondersteund door `naslagwerk`. Deze is nu los onder "raw" opgeslagen en moet handmatig doorgekopieerd worden naar "docs" indien het naslagwerk opnieuw gerendered wordt.
</commit_message>
<xml_diff>
--- a/topography.xlsx
+++ b/topography.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="191">
   <si>
     <t>section_order</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>c246f17d</t>
+  </si>
+  <si>
+    <t>1c667f9a</t>
   </si>
   <si>
     <t>3Ha14</t>
@@ -941,7 +944,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -987,7 +990,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -999,7 +1002,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1010,7 +1013,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1022,7 +1025,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1033,7 +1036,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1045,10 +1048,10 @@
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1059,7 +1062,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1071,10 +1074,10 @@
         <v>3</v>
       </c>
       <c r="I5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1085,7 +1088,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1097,10 +1100,10 @@
         <v>4</v>
       </c>
       <c r="I6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1111,7 +1114,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1123,10 +1126,10 @@
         <v>5</v>
       </c>
       <c r="I7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1137,7 +1140,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1149,10 +1152,10 @@
         <v>6</v>
       </c>
       <c r="I8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1163,7 +1166,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1175,10 +1178,10 @@
         <v>7</v>
       </c>
       <c r="I9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1189,7 +1192,7 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1198,13 +1201,13 @@
         <v>2</v>
       </c>
       <c r="G10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1215,7 +1218,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1224,13 +1227,13 @@
         <v>2</v>
       </c>
       <c r="G11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H11">
         <v>2</v>
       </c>
       <c r="I11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1241,7 +1244,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1250,13 +1253,13 @@
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H12">
         <v>3</v>
       </c>
       <c r="I12" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1267,7 +1270,7 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1276,13 +1279,13 @@
         <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H13">
         <v>4</v>
       </c>
       <c r="I13" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1293,7 +1296,7 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1305,10 +1308,7 @@
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>109</v>
-      </c>
-      <c r="J14" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1319,7 +1319,7 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1331,6 +1331,9 @@
         <v>2</v>
       </c>
       <c r="I15" t="s">
+        <v>110</v>
+      </c>
+      <c r="J15" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1342,7 +1345,7 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1362,7 +1365,7 @@
         <v>25</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
         <v>75</v>
@@ -1370,22 +1373,13 @@
       <c r="D17">
         <v>1</v>
       </c>
-      <c r="E17" t="s">
-        <v>78</v>
-      </c>
       <c r="F17">
         <v>1</v>
       </c>
-      <c r="G17" t="s">
-        <v>83</v>
-      </c>
       <c r="H17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I17" t="s">
-        <v>112</v>
-      </c>
-      <c r="J17" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1397,22 +1391,22 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F18">
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I18" t="s">
         <v>113</v>
@@ -1429,22 +1423,22 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F19">
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I19" t="s">
         <v>114</v>
@@ -1461,22 +1455,22 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I20" t="s">
         <v>115</v>
@@ -1493,28 +1487,28 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G21" t="s">
         <v>84</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I21" t="s">
         <v>116</v>
       </c>
       <c r="J21" t="s">
-        <v>156</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1525,22 +1519,22 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F22">
         <v>2</v>
       </c>
       <c r="G22" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I22" t="s">
         <v>117</v>
@@ -1557,28 +1551,28 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G23" t="s">
         <v>85</v>
       </c>
       <c r="H23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I23" t="s">
         <v>118</v>
       </c>
       <c r="J23" t="s">
-        <v>118</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1589,19 +1583,19 @@
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24" t="s">
         <v>79</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G24" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -1610,7 +1604,7 @@
         <v>119</v>
       </c>
       <c r="J24" t="s">
-        <v>158</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1621,22 +1615,22 @@
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D25">
         <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F25">
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I25" t="s">
         <v>120</v>
@@ -1653,22 +1647,22 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D26">
         <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I26" t="s">
         <v>121</v>
@@ -1685,22 +1679,22 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D27">
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I27" t="s">
         <v>122</v>
@@ -1717,16 +1711,16 @@
         <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D28">
         <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G28" t="s">
         <v>87</v>
@@ -1738,7 +1732,7 @@
         <v>123</v>
       </c>
       <c r="J28" t="s">
-        <v>123</v>
+        <v>162</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1749,28 +1743,28 @@
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D29">
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F29">
         <v>3</v>
       </c>
       <c r="G29" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I29" t="s">
         <v>124</v>
       </c>
       <c r="J29" t="s">
-        <v>162</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1781,28 +1775,28 @@
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D30">
         <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F30">
         <v>3</v>
       </c>
       <c r="G30" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I30" t="s">
         <v>125</v>
       </c>
       <c r="J30" t="s">
-        <v>125</v>
+        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1813,22 +1807,22 @@
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E31" t="s">
         <v>80</v>
       </c>
       <c r="F31">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G31" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H31">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I31" t="s">
         <v>126</v>
@@ -1845,10 +1839,10 @@
         <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E32" t="s">
         <v>81</v>
@@ -1857,7 +1851,7 @@
         <v>1</v>
       </c>
       <c r="G32" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H32">
         <v>1</v>
@@ -1877,22 +1871,22 @@
         <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D33">
         <v>4</v>
       </c>
       <c r="E33" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F33">
         <v>1</v>
       </c>
       <c r="G33" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I33" t="s">
         <v>128</v>
@@ -1909,28 +1903,28 @@
         <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D34">
         <v>4</v>
       </c>
       <c r="E34" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F34">
         <v>1</v>
       </c>
       <c r="G34" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I34" t="s">
         <v>129</v>
       </c>
       <c r="J34" t="s">
-        <v>95</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1941,25 +1935,28 @@
         <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D35">
         <v>4</v>
       </c>
       <c r="E35" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G35" t="s">
         <v>89</v>
       </c>
       <c r="H35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I35" t="s">
         <v>130</v>
+      </c>
+      <c r="J35" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1967,19 +1964,19 @@
         <v>44</v>
       </c>
       <c r="B36">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C36" t="s">
         <v>76</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E36" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G36" t="s">
         <v>90</v>
@@ -1989,9 +1986,6 @@
       </c>
       <c r="I36" t="s">
         <v>131</v>
-      </c>
-      <c r="J36" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -2002,16 +1996,16 @@
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G37" t="s">
         <v>91</v>
@@ -2034,25 +2028,25 @@
         <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F38">
         <v>2</v>
       </c>
       <c r="G38" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I38" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="J38" t="s">
         <v>165</v>
@@ -2066,25 +2060,25 @@
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G39" t="s">
         <v>92</v>
       </c>
       <c r="H39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I39" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="J39" t="s">
         <v>166</v>
@@ -2098,16 +2092,16 @@
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F40">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G40" t="s">
         <v>93</v>
@@ -2130,19 +2124,19 @@
         <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E41" t="s">
         <v>79</v>
       </c>
       <c r="F41">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G41" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="H41">
         <v>1</v>
@@ -2162,19 +2156,19 @@
         <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D42">
         <v>2</v>
       </c>
       <c r="E42" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G42" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H42">
         <v>1</v>
@@ -2194,22 +2188,22 @@
         <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D43">
         <v>2</v>
       </c>
       <c r="E43" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F43">
         <v>2</v>
       </c>
       <c r="G43" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I43" t="s">
         <v>137</v>
@@ -2226,22 +2220,22 @@
         <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D44">
         <v>2</v>
       </c>
       <c r="E44" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F44">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G44" t="s">
         <v>87</v>
       </c>
       <c r="H44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I44" t="s">
         <v>138</v>
@@ -2258,22 +2252,22 @@
         <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D45">
         <v>2</v>
       </c>
       <c r="E45" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F45">
         <v>3</v>
       </c>
       <c r="G45" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I45" t="s">
         <v>139</v>
@@ -2290,22 +2284,22 @@
         <v>5</v>
       </c>
       <c r="C46" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D46">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E46" t="s">
         <v>80</v>
       </c>
       <c r="F46">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G46" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I46" t="s">
         <v>140</v>
@@ -2322,22 +2316,22 @@
         <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D47">
         <v>3</v>
       </c>
       <c r="E47" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F47">
         <v>1</v>
       </c>
       <c r="G47" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I47" t="s">
         <v>141</v>
@@ -2354,10 +2348,10 @@
         <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D48">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E48" t="s">
         <v>81</v>
@@ -2366,16 +2360,16 @@
         <v>1</v>
       </c>
       <c r="G48" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="H48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I48" t="s">
         <v>142</v>
       </c>
       <c r="J48" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2386,28 +2380,28 @@
         <v>5</v>
       </c>
       <c r="C49" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D49">
         <v>5</v>
       </c>
       <c r="E49" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I49" t="s">
         <v>143</v>
       </c>
       <c r="J49" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2418,25 +2412,25 @@
         <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D50">
         <v>5</v>
       </c>
       <c r="E50" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G50" t="s">
         <v>95</v>
       </c>
       <c r="H50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I50" t="s">
-        <v>95</v>
+        <v>144</v>
       </c>
       <c r="J50" t="s">
         <v>176</v>
@@ -2450,16 +2444,16 @@
         <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D51">
         <v>5</v>
       </c>
       <c r="E51" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F51">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G51" t="s">
         <v>96</v>
@@ -2468,7 +2462,7 @@
         <v>1</v>
       </c>
       <c r="I51" t="s">
-        <v>144</v>
+        <v>96</v>
       </c>
       <c r="J51" t="s">
         <v>177</v>
@@ -2482,22 +2476,22 @@
         <v>5</v>
       </c>
       <c r="C52" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D52">
         <v>5</v>
       </c>
       <c r="E52" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F52">
         <v>4</v>
       </c>
       <c r="G52" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I52" t="s">
         <v>145</v>
@@ -2514,22 +2508,22 @@
         <v>5</v>
       </c>
       <c r="C53" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D53">
         <v>5</v>
       </c>
       <c r="E53" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F53">
         <v>4</v>
       </c>
       <c r="G53" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H53">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I53" t="s">
         <v>146</v>
@@ -2546,22 +2540,22 @@
         <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D54">
         <v>5</v>
       </c>
       <c r="E54" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F54">
         <v>4</v>
       </c>
       <c r="G54" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H54">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I54" t="s">
         <v>147</v>
@@ -2575,25 +2569,25 @@
         <v>63</v>
       </c>
       <c r="B55">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C55" t="s">
         <v>77</v>
       </c>
       <c r="D55">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E55" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F55">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G55" t="s">
         <v>97</v>
       </c>
       <c r="H55">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I55" t="s">
         <v>148</v>
@@ -2610,22 +2604,22 @@
         <v>6</v>
       </c>
       <c r="C56" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D56">
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F56">
         <v>1</v>
       </c>
       <c r="G56" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I56" t="s">
         <v>149</v>
@@ -2642,22 +2636,22 @@
         <v>6</v>
       </c>
       <c r="C57" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D57">
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G57" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="H57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I57" t="s">
         <v>150</v>
@@ -2674,22 +2668,22 @@
         <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D58">
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F58">
         <v>2</v>
       </c>
       <c r="G58" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I58" t="s">
         <v>151</v>
@@ -2706,25 +2700,25 @@
         <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D59">
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F59">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G59" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I59" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="J59" t="s">
         <v>185</v>
@@ -2738,25 +2732,25 @@
         <v>6</v>
       </c>
       <c r="C60" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E60" t="s">
         <v>79</v>
       </c>
       <c r="F60">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G60" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="H60">
         <v>1</v>
       </c>
       <c r="I60" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="J60" t="s">
         <v>186</v>
@@ -2770,22 +2764,22 @@
         <v>6</v>
       </c>
       <c r="C61" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D61">
         <v>2</v>
       </c>
       <c r="E61" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F61">
         <v>1</v>
       </c>
       <c r="G61" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I61" t="s">
         <v>153</v>
@@ -2802,22 +2796,22 @@
         <v>6</v>
       </c>
       <c r="C62" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D62">
         <v>2</v>
       </c>
       <c r="E62" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F62">
         <v>1</v>
       </c>
       <c r="G62" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H62">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I62" t="s">
         <v>154</v>
@@ -2834,25 +2828,57 @@
         <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D63">
+        <v>2</v>
+      </c>
+      <c r="E63" t="s">
+        <v>80</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+      <c r="G63" t="s">
+        <v>91</v>
+      </c>
+      <c r="H63">
         <v>3</v>
-      </c>
-      <c r="E63" t="s">
-        <v>81</v>
-      </c>
-      <c r="F63">
-        <v>1</v>
-      </c>
-      <c r="H63">
-        <v>1</v>
       </c>
       <c r="I63" t="s">
         <v>155</v>
       </c>
       <c r="J63" t="s">
         <v>189</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B64">
+        <v>6</v>
+      </c>
+      <c r="C64" t="s">
+        <v>78</v>
+      </c>
+      <c r="D64">
+        <v>3</v>
+      </c>
+      <c r="E64" t="s">
+        <v>82</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64" t="s">
+        <v>156</v>
+      </c>
+      <c r="J64" t="s">
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Verwijderen pagina "individueel matchen"
Het doel van deze pagina was niet duidelijk. Er kan volstaan worden met de pagina "individueel uitnodigen". Deze is al aangepast zodat het de lading van de verwijderde pagina ook dekt.

Zie: 510ba61ce988331d20fd0849a65354003586e46d
</commit_message>
<xml_diff>
--- a/topography.xlsx
+++ b/topography.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\UBD\FCA\ASC\05. CSA\80. Naslagwerken\matching\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68F2E2E-EB58-406F-850B-ED6142248461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-28920" yWindow="-8820" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site_topography" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="188">
   <si>
     <t>section_order</t>
   </si>
@@ -121,9 +127,6 @@
     <t>dZH9V</t>
   </si>
   <si>
-    <t>UjWU9</t>
-  </si>
-  <si>
     <t>qOuQE</t>
   </si>
   <si>
@@ -382,9 +385,6 @@
     <t>Individueel uitnodigen</t>
   </si>
   <si>
-    <t>Individuele matching</t>
-  </si>
-  <si>
     <t>Verwerken verzoek</t>
   </si>
   <si>
@@ -497,9 +497,6 @@
   </si>
   <si>
     <t>Individueel uitnodigen activiteit</t>
-  </si>
-  <si>
-    <t>Uitnodigen individuele matching</t>
   </si>
   <si>
     <t>Verwerken verzoek alternatieve datum</t>
@@ -592,8 +589,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -656,13 +653,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -700,7 +705,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -734,6 +739,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -768,9 +774,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -943,14 +950,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:XFD27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="40.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -982,7 +1003,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -990,7 +1011,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1002,10 +1023,10 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1013,7 +1034,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1025,10 +1046,10 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1036,7 +1057,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1048,13 +1069,13 @@
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1062,7 +1083,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1074,13 +1095,13 @@
         <v>3</v>
       </c>
       <c r="I5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -1088,7 +1109,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1100,13 +1121,13 @@
         <v>4</v>
       </c>
       <c r="I6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1114,7 +1135,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1126,13 +1147,13 @@
         <v>5</v>
       </c>
       <c r="I7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1140,7 +1161,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1152,13 +1173,13 @@
         <v>6</v>
       </c>
       <c r="I8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -1166,7 +1187,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1178,13 +1199,13 @@
         <v>7</v>
       </c>
       <c r="I9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -1192,7 +1213,7 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1201,16 +1222,16 @@
         <v>2</v>
       </c>
       <c r="G10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1218,7 +1239,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1227,16 +1248,16 @@
         <v>2</v>
       </c>
       <c r="G11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H11">
         <v>2</v>
       </c>
       <c r="I11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -1244,7 +1265,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1253,16 +1274,16 @@
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H12">
         <v>3</v>
       </c>
       <c r="I12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
@@ -1270,7 +1291,7 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1279,16 +1300,16 @@
         <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H13">
         <v>4</v>
       </c>
       <c r="I13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -1296,7 +1317,7 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1308,10 +1329,10 @@
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1319,7 +1340,7 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1331,13 +1352,13 @@
         <v>2</v>
       </c>
       <c r="I15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -1345,7 +1366,7 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1357,10 +1378,10 @@
         <v>3</v>
       </c>
       <c r="I16" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -1368,7 +1389,7 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1380,10 +1401,10 @@
         <v>4</v>
       </c>
       <c r="I17" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -1391,31 +1412,31 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F18">
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H18">
         <v>1</v>
       </c>
       <c r="I18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J18" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
@@ -1423,31 +1444,31 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F19">
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H19">
         <v>2</v>
       </c>
       <c r="I19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J19" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
@@ -1455,31 +1476,31 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H20">
         <v>3</v>
       </c>
       <c r="I20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J20" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
@@ -1487,31 +1508,31 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F21">
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H21">
         <v>4</v>
       </c>
       <c r="I21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J21" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -1519,31 +1540,31 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F22">
         <v>2</v>
       </c>
       <c r="G22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H22">
         <v>1</v>
       </c>
       <c r="I22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J22" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>31</v>
       </c>
@@ -1551,31 +1572,31 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F23">
         <v>2</v>
       </c>
       <c r="G23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H23">
         <v>2</v>
       </c>
       <c r="I23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J23" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
@@ -1583,31 +1604,31 @@
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F24">
         <v>3</v>
       </c>
       <c r="G24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H24">
         <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J24" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
@@ -1615,31 +1636,31 @@
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D25">
         <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F25">
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H25">
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J25" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
@@ -1647,31 +1668,31 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D26">
         <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H26">
         <v>2</v>
       </c>
       <c r="I26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J26" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>35</v>
       </c>
@@ -1679,31 +1700,31 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D27">
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G27" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J27" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
@@ -1711,16 +1732,16 @@
         <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D28">
         <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G28" t="s">
         <v>87</v>
@@ -1729,13 +1750,13 @@
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J28" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>37</v>
       </c>
@@ -1743,31 +1764,31 @@
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D29">
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F29">
         <v>3</v>
       </c>
       <c r="G29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J29" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
@@ -1775,31 +1796,31 @@
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D30">
         <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F30">
         <v>3</v>
       </c>
       <c r="G30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J30" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>39</v>
       </c>
@@ -1807,31 +1828,31 @@
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E31" t="s">
         <v>80</v>
       </c>
       <c r="F31">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G31" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H31">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J31" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>40</v>
       </c>
@@ -1839,10 +1860,10 @@
         <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E32" t="s">
         <v>81</v>
@@ -1851,19 +1872,19 @@
         <v>1</v>
       </c>
       <c r="G32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H32">
         <v>1</v>
       </c>
       <c r="I32" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J32" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>41</v>
       </c>
@@ -1871,31 +1892,31 @@
         <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D33">
         <v>4</v>
       </c>
       <c r="E33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F33">
         <v>1</v>
       </c>
       <c r="G33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J33" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>42</v>
       </c>
@@ -1903,31 +1924,31 @@
         <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D34">
         <v>4</v>
       </c>
       <c r="E34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F34">
         <v>1</v>
       </c>
       <c r="G34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J34" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>43</v>
       </c>
@@ -1935,48 +1956,45 @@
         <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D35">
         <v>4</v>
       </c>
       <c r="E35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G35" t="s">
         <v>89</v>
       </c>
       <c r="H35">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I35" t="s">
-        <v>130</v>
-      </c>
-      <c r="J35" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B36">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s">
         <v>76</v>
       </c>
       <c r="D36">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G36" t="s">
         <v>90</v>
@@ -1985,10 +2003,13 @@
         <v>1</v>
       </c>
       <c r="I36" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10">
+        <v>130</v>
+      </c>
+      <c r="J36" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>45</v>
       </c>
@@ -1996,16 +2017,16 @@
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G37" t="s">
         <v>91</v>
@@ -2014,13 +2035,13 @@
         <v>1</v>
       </c>
       <c r="I37" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J37" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>46</v>
       </c>
@@ -2028,31 +2049,31 @@
         <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F38">
         <v>2</v>
       </c>
       <c r="G38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I38" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="J38" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>47</v>
       </c>
@@ -2060,31 +2081,31 @@
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F39">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G39" t="s">
         <v>92</v>
       </c>
       <c r="H39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I39" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="J39" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>48</v>
       </c>
@@ -2092,16 +2113,16 @@
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F40">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G40" t="s">
         <v>93</v>
@@ -2110,13 +2131,13 @@
         <v>1</v>
       </c>
       <c r="I40" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J40" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>49</v>
       </c>
@@ -2124,31 +2145,31 @@
         <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E41" t="s">
         <v>79</v>
       </c>
       <c r="F41">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G41" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="H41">
         <v>1</v>
       </c>
       <c r="I41" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J41" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>50</v>
       </c>
@@ -2156,31 +2177,31 @@
         <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D42">
         <v>2</v>
       </c>
       <c r="E42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G42" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H42">
         <v>1</v>
       </c>
       <c r="I42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J42" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>51</v>
       </c>
@@ -2188,31 +2209,31 @@
         <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D43">
         <v>2</v>
       </c>
       <c r="E43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F43">
         <v>2</v>
       </c>
       <c r="G43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I43" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J43" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>52</v>
       </c>
@@ -2220,31 +2241,31 @@
         <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D44">
         <v>2</v>
       </c>
       <c r="E44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F44">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G44" t="s">
         <v>87</v>
       </c>
       <c r="H44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I44" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J44" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>53</v>
       </c>
@@ -2252,31 +2273,31 @@
         <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D45">
         <v>2</v>
       </c>
       <c r="E45" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F45">
         <v>3</v>
       </c>
       <c r="G45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I45" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J45" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>54</v>
       </c>
@@ -2284,31 +2305,31 @@
         <v>5</v>
       </c>
       <c r="C46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D46">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E46" t="s">
         <v>80</v>
       </c>
       <c r="F46">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G46" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I46" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J46" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>55</v>
       </c>
@@ -2316,31 +2337,31 @@
         <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D47">
         <v>3</v>
       </c>
       <c r="E47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F47">
         <v>1</v>
       </c>
       <c r="G47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J47" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>56</v>
       </c>
@@ -2348,10 +2369,10 @@
         <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D48">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E48" t="s">
         <v>81</v>
@@ -2360,19 +2381,19 @@
         <v>1</v>
       </c>
       <c r="G48" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="H48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I48" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J48" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>57</v>
       </c>
@@ -2380,31 +2401,31 @@
         <v>5</v>
       </c>
       <c r="C49" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D49">
         <v>5</v>
       </c>
       <c r="E49" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G49" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I49" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J49" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>58</v>
       </c>
@@ -2412,31 +2433,31 @@
         <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D50">
         <v>5</v>
       </c>
       <c r="E50" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F50">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G50" t="s">
         <v>95</v>
       </c>
       <c r="H50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I50" t="s">
-        <v>144</v>
+        <v>95</v>
       </c>
       <c r="J50" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>59</v>
       </c>
@@ -2444,16 +2465,16 @@
         <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D51">
         <v>5</v>
       </c>
       <c r="E51" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F51">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G51" t="s">
         <v>96</v>
@@ -2462,13 +2483,13 @@
         <v>1</v>
       </c>
       <c r="I51" t="s">
-        <v>96</v>
+        <v>143</v>
       </c>
       <c r="J51" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>60</v>
       </c>
@@ -2476,31 +2497,31 @@
         <v>5</v>
       </c>
       <c r="C52" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D52">
         <v>5</v>
       </c>
       <c r="E52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F52">
         <v>4</v>
       </c>
       <c r="G52" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I52" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J52" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>61</v>
       </c>
@@ -2508,31 +2529,31 @@
         <v>5</v>
       </c>
       <c r="C53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D53">
         <v>5</v>
       </c>
       <c r="E53" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F53">
         <v>4</v>
       </c>
       <c r="G53" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H53">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I53" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J53" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>62</v>
       </c>
@@ -2540,63 +2561,63 @@
         <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D54">
         <v>5</v>
       </c>
       <c r="E54" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F54">
         <v>4</v>
       </c>
       <c r="G54" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H54">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I54" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J54" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B55">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C55" t="s">
         <v>77</v>
       </c>
       <c r="D55">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F55">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G55" t="s">
         <v>97</v>
       </c>
       <c r="H55">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I55" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J55" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>64</v>
       </c>
@@ -2604,31 +2625,31 @@
         <v>6</v>
       </c>
       <c r="C56" t="s">
+        <v>77</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56" t="s">
         <v>78</v>
       </c>
-      <c r="D56">
-        <v>1</v>
-      </c>
-      <c r="E56" t="s">
-        <v>79</v>
-      </c>
       <c r="F56">
         <v>1</v>
       </c>
       <c r="G56" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I56" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J56" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>65</v>
       </c>
@@ -2636,31 +2657,31 @@
         <v>6</v>
       </c>
       <c r="C57" t="s">
+        <v>77</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57" t="s">
         <v>78</v>
       </c>
-      <c r="D57">
-        <v>1</v>
-      </c>
-      <c r="E57" t="s">
-        <v>79</v>
-      </c>
       <c r="F57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G57" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="H57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I57" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J57" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>66</v>
       </c>
@@ -2668,31 +2689,31 @@
         <v>6</v>
       </c>
       <c r="C58" t="s">
+        <v>77</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58" t="s">
         <v>78</v>
       </c>
-      <c r="D58">
-        <v>1</v>
-      </c>
-      <c r="E58" t="s">
-        <v>79</v>
-      </c>
       <c r="F58">
         <v>2</v>
       </c>
       <c r="G58" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I58" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J58" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>67</v>
       </c>
@@ -2700,31 +2721,31 @@
         <v>6</v>
       </c>
       <c r="C59" t="s">
+        <v>77</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59" t="s">
         <v>78</v>
       </c>
-      <c r="D59">
-        <v>1</v>
-      </c>
-      <c r="E59" t="s">
-        <v>79</v>
-      </c>
       <c r="F59">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G59" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I59" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="J59" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>68</v>
       </c>
@@ -2732,31 +2753,31 @@
         <v>6</v>
       </c>
       <c r="C60" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E60" t="s">
         <v>79</v>
       </c>
       <c r="F60">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G60" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H60">
         <v>1</v>
       </c>
       <c r="I60" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="J60" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>69</v>
       </c>
@@ -2764,31 +2785,31 @@
         <v>6</v>
       </c>
       <c r="C61" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D61">
         <v>2</v>
       </c>
       <c r="E61" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F61">
         <v>1</v>
       </c>
       <c r="G61" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I61" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J61" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>70</v>
       </c>
@@ -2796,31 +2817,31 @@
         <v>6</v>
       </c>
       <c r="C62" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D62">
         <v>2</v>
       </c>
       <c r="E62" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F62">
         <v>1</v>
       </c>
       <c r="G62" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H62">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I62" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J62" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>71</v>
       </c>
@@ -2828,57 +2849,25 @@
         <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D63">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E63" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F63">
         <v>1</v>
       </c>
-      <c r="G63" t="s">
-        <v>91</v>
-      </c>
       <c r="H63">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I63" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J63" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10">
-      <c r="A64" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B64">
-        <v>6</v>
-      </c>
-      <c r="C64" t="s">
-        <v>78</v>
-      </c>
-      <c r="D64">
-        <v>3</v>
-      </c>
-      <c r="E64" t="s">
-        <v>82</v>
-      </c>
-      <c r="F64">
-        <v>1</v>
-      </c>
-      <c r="H64">
-        <v>1</v>
-      </c>
-      <c r="I64" t="s">
-        <v>156</v>
-      </c>
-      <c r="J64" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Verwijder bronbestand "individuele matching"
Zie 5f53354b6eff6571d2dc257a067e2d9fa4bc612c
</commit_message>
<xml_diff>
--- a/topography.xlsx
+++ b/topography.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\UBD\FCA\ASC\05. CSA\80. Naslagwerken\matching\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68F2E2E-EB58-406F-850B-ED6142248461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-8820" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="site_topography" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -589,8 +583,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -653,21 +647,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -705,7 +691,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -739,7 +725,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -774,10 +759,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -950,28 +934,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:XFD27"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="42.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="40.6640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1003,7 +973,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1026,7 +996,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1049,7 +1019,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1075,7 +1045,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1101,7 +1071,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -1127,7 +1097,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1153,7 +1123,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1179,7 +1149,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -1205,7 +1175,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -1231,7 +1201,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1257,7 +1227,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -1283,7 +1253,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
@@ -1309,7 +1279,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -1332,7 +1302,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1358,7 +1328,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -1381,7 +1351,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -1404,7 +1374,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -1436,7 +1406,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
@@ -1468,7 +1438,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
@@ -1500,7 +1470,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
@@ -1532,7 +1502,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -1564,7 +1534,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
         <v>31</v>
       </c>
@@ -1596,7 +1566,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
@@ -1628,7 +1598,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
@@ -1660,7 +1630,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
@@ -1692,7 +1662,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
         <v>35</v>
       </c>
@@ -1724,7 +1694,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
@@ -1756,7 +1726,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
         <v>37</v>
       </c>
@@ -1788,7 +1758,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
@@ -1820,7 +1790,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
         <v>39</v>
       </c>
@@ -1852,7 +1822,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
         <v>40</v>
       </c>
@@ -1884,7 +1854,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
         <v>41</v>
       </c>
@@ -1916,7 +1886,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
         <v>42</v>
       </c>
@@ -1948,7 +1918,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
         <v>43</v>
       </c>
@@ -1977,7 +1947,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10">
       <c r="A36" s="1" t="s">
         <v>44</v>
       </c>
@@ -2009,7 +1979,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10">
       <c r="A37" s="1" t="s">
         <v>45</v>
       </c>
@@ -2041,7 +2011,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10">
       <c r="A38" s="1" t="s">
         <v>46</v>
       </c>
@@ -2073,7 +2043,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10">
       <c r="A39" s="1" t="s">
         <v>47</v>
       </c>
@@ -2105,7 +2075,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10">
       <c r="A40" s="1" t="s">
         <v>48</v>
       </c>
@@ -2137,7 +2107,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10">
       <c r="A41" s="1" t="s">
         <v>49</v>
       </c>
@@ -2169,7 +2139,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10">
       <c r="A42" s="1" t="s">
         <v>50</v>
       </c>
@@ -2201,7 +2171,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10">
       <c r="A43" s="1" t="s">
         <v>51</v>
       </c>
@@ -2233,7 +2203,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10">
       <c r="A44" s="1" t="s">
         <v>52</v>
       </c>
@@ -2265,7 +2235,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10">
       <c r="A45" s="1" t="s">
         <v>53</v>
       </c>
@@ -2297,7 +2267,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10">
       <c r="A46" s="1" t="s">
         <v>54</v>
       </c>
@@ -2329,7 +2299,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10">
       <c r="A47" s="1" t="s">
         <v>55</v>
       </c>
@@ -2361,7 +2331,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10">
       <c r="A48" s="1" t="s">
         <v>56</v>
       </c>
@@ -2393,7 +2363,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10">
       <c r="A49" s="1" t="s">
         <v>57</v>
       </c>
@@ -2425,7 +2395,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10">
       <c r="A50" s="1" t="s">
         <v>58</v>
       </c>
@@ -2457,7 +2427,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10">
       <c r="A51" s="1" t="s">
         <v>59</v>
       </c>
@@ -2489,7 +2459,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10">
       <c r="A52" s="1" t="s">
         <v>60</v>
       </c>
@@ -2521,7 +2491,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10">
       <c r="A53" s="1" t="s">
         <v>61</v>
       </c>
@@ -2553,7 +2523,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10">
       <c r="A54" s="1" t="s">
         <v>62</v>
       </c>
@@ -2585,7 +2555,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10">
       <c r="A55" s="1" t="s">
         <v>63</v>
       </c>
@@ -2617,7 +2587,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10">
       <c r="A56" s="1" t="s">
         <v>64</v>
       </c>
@@ -2649,7 +2619,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10">
       <c r="A57" s="1" t="s">
         <v>65</v>
       </c>
@@ -2681,7 +2651,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10">
       <c r="A58" s="1" t="s">
         <v>66</v>
       </c>
@@ -2713,7 +2683,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10">
       <c r="A59" s="1" t="s">
         <v>67</v>
       </c>
@@ -2745,7 +2715,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10">
       <c r="A60" s="1" t="s">
         <v>68</v>
       </c>
@@ -2777,7 +2747,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10">
       <c r="A61" s="1" t="s">
         <v>69</v>
       </c>
@@ -2809,7 +2779,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10">
       <c r="A62" s="1" t="s">
         <v>70</v>
       </c>
@@ -2841,7 +2811,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10">
       <c r="A63" s="1" t="s">
         <v>71</v>
       </c>

</xml_diff>

<commit_message>
Prepareer nieuwe versie naslagwerk
- Kleur aangepast
- Titel aangepast
- Versie nummer aangepast
- Changelog pagina toegevoegd
- Pagina individuele matching verwijderd
</commit_message>
<xml_diff>
--- a/topography.xlsx
+++ b/topography.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="190">
   <si>
     <t>section_order</t>
   </si>
@@ -49,6 +49,9 @@
     <t>Ueh68</t>
   </si>
   <si>
+    <t>265e3b99</t>
+  </si>
+  <si>
     <t>Jf034</t>
   </si>
   <si>
@@ -308,6 +311,9 @@
   </si>
   <si>
     <t>Processtart</t>
+  </si>
+  <si>
+    <t>Changelog</t>
   </si>
   <si>
     <t>Wijzigingen</t>
@@ -935,7 +941,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -981,7 +987,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -993,7 +999,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1001,7 +1007,7 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>73</v>
@@ -1013,10 +1019,10 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1027,7 +1033,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1036,13 +1042,10 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>99</v>
-      </c>
-      <c r="J4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1053,7 +1056,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1062,13 +1065,13 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1079,7 +1082,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1088,13 +1091,13 @@
         <v>1</v>
       </c>
       <c r="H6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1105,7 +1108,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1114,13 +1117,13 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1131,7 +1134,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1140,13 +1143,13 @@
         <v>1</v>
       </c>
       <c r="H8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1157,7 +1160,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1166,13 +1169,13 @@
         <v>1</v>
       </c>
       <c r="H9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1183,22 +1186,22 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="F10">
-        <v>2</v>
-      </c>
-      <c r="G10" t="s">
-        <v>82</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I10" t="s">
-        <v>105</v>
+        <v>106</v>
+      </c>
+      <c r="J10" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1209,7 +1212,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1218,13 +1221,13 @@
         <v>2</v>
       </c>
       <c r="G11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1235,7 +1238,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1244,13 +1247,13 @@
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I12" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1261,7 +1264,7 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1270,13 +1273,13 @@
         <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I13" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1284,7 +1287,7 @@
         <v>22</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
         <v>74</v>
@@ -1293,13 +1296,16 @@
         <v>1</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G14" t="s">
+        <v>83</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I14" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1310,7 +1316,7 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1319,13 +1325,10 @@
         <v>1</v>
       </c>
       <c r="H15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>109</v>
-      </c>
-      <c r="J15" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1336,7 +1339,7 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1345,10 +1348,13 @@
         <v>1</v>
       </c>
       <c r="H16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I16" t="s">
-        <v>110</v>
+        <v>111</v>
+      </c>
+      <c r="J16" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1359,7 +1365,7 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1368,10 +1374,10 @@
         <v>1</v>
       </c>
       <c r="H17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1379,7 +1385,7 @@
         <v>26</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
         <v>75</v>
@@ -1387,23 +1393,14 @@
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="E18" t="s">
-        <v>78</v>
-      </c>
       <c r="F18">
         <v>1</v>
       </c>
-      <c r="G18" t="s">
-        <v>83</v>
-      </c>
       <c r="H18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I18" t="s">
-        <v>112</v>
-      </c>
-      <c r="J18" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1414,28 +1411,28 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F19">
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I19" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J19" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1446,28 +1443,28 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I20" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J20" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1478,28 +1475,28 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F21">
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I21" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J21" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1510,28 +1507,28 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G22" t="s">
         <v>84</v>
       </c>
       <c r="H22">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I22" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J22" t="s">
-        <v>155</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1542,28 +1539,28 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F23">
         <v>2</v>
       </c>
       <c r="G23" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I23" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J23" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1574,28 +1571,28 @@
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G24" t="s">
         <v>85</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I24" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J24" t="s">
-        <v>118</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1606,28 +1603,28 @@
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25" t="s">
         <v>79</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G25" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H25">
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J25" t="s">
-        <v>157</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1638,28 +1635,28 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D26">
         <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I26" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J26" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1670,28 +1667,28 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D27">
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I27" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J27" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1702,16 +1699,16 @@
         <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D28">
         <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G28" t="s">
         <v>87</v>
@@ -1720,10 +1717,10 @@
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J28" t="s">
-        <v>122</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1734,28 +1731,28 @@
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D29">
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F29">
         <v>3</v>
       </c>
       <c r="G29" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I29" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J29" t="s">
-        <v>160</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1766,28 +1763,28 @@
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D30">
         <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F30">
         <v>3</v>
       </c>
       <c r="G30" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I30" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J30" t="s">
-        <v>124</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1798,28 +1795,28 @@
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E31" t="s">
         <v>80</v>
       </c>
       <c r="F31">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G31" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H31">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I31" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J31" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1830,10 +1827,10 @@
         <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E32" t="s">
         <v>81</v>
@@ -1842,16 +1839,16 @@
         <v>1</v>
       </c>
       <c r="G32" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H32">
         <v>1</v>
       </c>
       <c r="I32" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="J32" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1862,28 +1859,28 @@
         <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D33">
         <v>4</v>
       </c>
       <c r="E33" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F33">
         <v>1</v>
       </c>
       <c r="G33" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I33" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="J33" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1894,28 +1891,28 @@
         <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D34">
         <v>4</v>
       </c>
       <c r="E34" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F34">
         <v>1</v>
       </c>
       <c r="G34" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I34" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J34" t="s">
-        <v>95</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1926,25 +1923,28 @@
         <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D35">
         <v>4</v>
       </c>
       <c r="E35" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G35" t="s">
         <v>89</v>
       </c>
       <c r="H35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I35" t="s">
-        <v>129</v>
+        <v>130</v>
+      </c>
+      <c r="J35" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1952,19 +1952,19 @@
         <v>44</v>
       </c>
       <c r="B36">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C36" t="s">
         <v>76</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E36" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G36" t="s">
         <v>90</v>
@@ -1973,10 +1973,7 @@
         <v>1</v>
       </c>
       <c r="I36" t="s">
-        <v>130</v>
-      </c>
-      <c r="J36" t="s">
-        <v>161</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -1987,16 +1984,16 @@
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G37" t="s">
         <v>91</v>
@@ -2005,10 +2002,10 @@
         <v>1</v>
       </c>
       <c r="I37" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J37" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -2019,28 +2016,28 @@
         <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F38">
         <v>2</v>
       </c>
       <c r="G38" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I38" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="J38" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2051,28 +2048,28 @@
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G39" t="s">
         <v>92</v>
       </c>
       <c r="H39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I39" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="J39" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -2083,16 +2080,16 @@
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F40">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G40" t="s">
         <v>93</v>
@@ -2101,10 +2098,10 @@
         <v>1</v>
       </c>
       <c r="I40" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J40" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2115,28 +2112,28 @@
         <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E41" t="s">
         <v>79</v>
       </c>
       <c r="F41">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G41" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="H41">
         <v>1</v>
       </c>
       <c r="I41" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="J41" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2147,28 +2144,28 @@
         <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D42">
         <v>2</v>
       </c>
       <c r="E42" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G42" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H42">
         <v>1</v>
       </c>
       <c r="I42" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="J42" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -2179,28 +2176,28 @@
         <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D43">
         <v>2</v>
       </c>
       <c r="E43" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F43">
         <v>2</v>
       </c>
       <c r="G43" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I43" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J43" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -2211,28 +2208,28 @@
         <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D44">
         <v>2</v>
       </c>
       <c r="E44" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F44">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G44" t="s">
         <v>87</v>
       </c>
       <c r="H44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I44" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="J44" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2243,28 +2240,28 @@
         <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D45">
         <v>2</v>
       </c>
       <c r="E45" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F45">
         <v>3</v>
       </c>
       <c r="G45" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I45" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J45" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2275,28 +2272,28 @@
         <v>5</v>
       </c>
       <c r="C46" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D46">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E46" t="s">
         <v>80</v>
       </c>
       <c r="F46">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G46" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I46" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J46" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2307,28 +2304,28 @@
         <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D47">
         <v>3</v>
       </c>
       <c r="E47" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F47">
         <v>1</v>
       </c>
       <c r="G47" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I47" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J47" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -2339,10 +2336,10 @@
         <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D48">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E48" t="s">
         <v>81</v>
@@ -2351,16 +2348,16 @@
         <v>1</v>
       </c>
       <c r="G48" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="H48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I48" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J48" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2371,28 +2368,28 @@
         <v>5</v>
       </c>
       <c r="C49" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D49">
         <v>5</v>
       </c>
       <c r="E49" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I49" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="J49" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2403,28 +2400,28 @@
         <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D50">
         <v>5</v>
       </c>
       <c r="E50" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G50" t="s">
         <v>95</v>
       </c>
       <c r="H50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I50" t="s">
-        <v>95</v>
+        <v>144</v>
       </c>
       <c r="J50" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2435,16 +2432,16 @@
         <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D51">
         <v>5</v>
       </c>
       <c r="E51" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F51">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G51" t="s">
         <v>96</v>
@@ -2453,10 +2450,10 @@
         <v>1</v>
       </c>
       <c r="I51" t="s">
-        <v>143</v>
+        <v>96</v>
       </c>
       <c r="J51" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2467,28 +2464,28 @@
         <v>5</v>
       </c>
       <c r="C52" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D52">
         <v>5</v>
       </c>
       <c r="E52" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F52">
         <v>4</v>
       </c>
       <c r="G52" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I52" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J52" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2499,28 +2496,28 @@
         <v>5</v>
       </c>
       <c r="C53" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D53">
         <v>5</v>
       </c>
       <c r="E53" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F53">
         <v>4</v>
       </c>
       <c r="G53" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H53">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I53" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="J53" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2531,28 +2528,28 @@
         <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D54">
         <v>5</v>
       </c>
       <c r="E54" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F54">
         <v>4</v>
       </c>
       <c r="G54" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H54">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I54" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J54" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2560,31 +2557,31 @@
         <v>63</v>
       </c>
       <c r="B55">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C55" t="s">
         <v>77</v>
       </c>
       <c r="D55">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E55" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F55">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G55" t="s">
         <v>97</v>
       </c>
       <c r="H55">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I55" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J55" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -2595,28 +2592,28 @@
         <v>6</v>
       </c>
       <c r="C56" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D56">
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F56">
         <v>1</v>
       </c>
       <c r="G56" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I56" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J56" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2627,28 +2624,28 @@
         <v>6</v>
       </c>
       <c r="C57" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D57">
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G57" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="H57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I57" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J57" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -2659,28 +2656,28 @@
         <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D58">
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F58">
         <v>2</v>
       </c>
       <c r="G58" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I58" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="J58" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -2691,28 +2688,28 @@
         <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D59">
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F59">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G59" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I59" t="s">
-        <v>133</v>
+        <v>152</v>
       </c>
       <c r="J59" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -2723,28 +2720,28 @@
         <v>6</v>
       </c>
       <c r="C60" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E60" t="s">
         <v>79</v>
       </c>
       <c r="F60">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G60" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="H60">
         <v>1</v>
       </c>
       <c r="I60" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="J60" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -2755,28 +2752,28 @@
         <v>6</v>
       </c>
       <c r="C61" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D61">
         <v>2</v>
       </c>
       <c r="E61" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F61">
         <v>1</v>
       </c>
       <c r="G61" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I61" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="J61" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -2787,28 +2784,28 @@
         <v>6</v>
       </c>
       <c r="C62" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D62">
         <v>2</v>
       </c>
       <c r="E62" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F62">
         <v>1</v>
       </c>
       <c r="G62" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H62">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I62" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J62" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -2819,25 +2816,57 @@
         <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D63">
+        <v>2</v>
+      </c>
+      <c r="E63" t="s">
+        <v>80</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+      <c r="G63" t="s">
+        <v>91</v>
+      </c>
+      <c r="H63">
         <v>3</v>
       </c>
-      <c r="E63" t="s">
-        <v>81</v>
-      </c>
-      <c r="F63">
-        <v>1</v>
-      </c>
-      <c r="H63">
-        <v>1</v>
-      </c>
       <c r="I63" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="J63" t="s">
-        <v>187</v>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B64">
+        <v>6</v>
+      </c>
+      <c r="C64" t="s">
+        <v>78</v>
+      </c>
+      <c r="D64">
+        <v>3</v>
+      </c>
+      <c r="E64" t="s">
+        <v>82</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64" t="s">
+        <v>156</v>
+      </c>
+      <c r="J64" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Verwerken verzoek - Aanpassing rubrieksnaam (kleine tekstuele aanpassing)
Nieuwe pagina toegevoegd met instrucutie individueel registreren aanwezigheid
</commit_message>
<xml_diff>
--- a/topography.xlsx
+++ b/topography.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="193">
   <si>
     <t>section_order</t>
   </si>
@@ -136,6 +136,9 @@
     <t>urZgR</t>
   </si>
   <si>
+    <t>f7715b38</t>
+  </si>
+  <si>
     <t>EuZ4y</t>
   </si>
   <si>
@@ -397,6 +400,9 @@
     <t>Inlezen presentielijst</t>
   </si>
   <si>
+    <t>Registeren aanwezigheid (individueel)</t>
+  </si>
+  <si>
     <t>Afwijzen te late aanmelders</t>
   </si>
   <si>
@@ -503,6 +509,9 @@
   </si>
   <si>
     <t>Conversie presentielijst</t>
+  </si>
+  <si>
+    <t>Registreren aanwezigheid individueel</t>
   </si>
   <si>
     <t>M-FOR-U-****</t>
@@ -941,7 +950,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J64"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -987,7 +996,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -999,7 +1008,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1010,7 +1019,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1022,7 +1031,7 @@
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1033,7 +1042,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1045,7 +1054,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1056,7 +1065,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1068,10 +1077,10 @@
         <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1082,7 +1091,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1094,10 +1103,10 @@
         <v>3</v>
       </c>
       <c r="I6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1108,7 +1117,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1120,10 +1129,10 @@
         <v>4</v>
       </c>
       <c r="I7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1134,7 +1143,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1146,10 +1155,10 @@
         <v>5</v>
       </c>
       <c r="I8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1160,7 +1169,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1172,10 +1181,10 @@
         <v>6</v>
       </c>
       <c r="I9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1186,7 +1195,7 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1198,10 +1207,10 @@
         <v>7</v>
       </c>
       <c r="I10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1212,7 +1221,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1221,13 +1230,13 @@
         <v>2</v>
       </c>
       <c r="G11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H11">
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1238,7 +1247,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1247,13 +1256,13 @@
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H12">
         <v>2</v>
       </c>
       <c r="I12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1264,7 +1273,7 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1273,13 +1282,13 @@
         <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H13">
         <v>3</v>
       </c>
       <c r="I13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1290,7 +1299,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1299,13 +1308,13 @@
         <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H14">
         <v>4</v>
       </c>
       <c r="I14" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1316,7 +1325,7 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1328,7 +1337,7 @@
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1339,7 +1348,7 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1351,10 +1360,10 @@
         <v>2</v>
       </c>
       <c r="I16" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J16" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1365,7 +1374,7 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1377,7 +1386,7 @@
         <v>3</v>
       </c>
       <c r="I17" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1388,7 +1397,7 @@
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1400,7 +1409,7 @@
         <v>4</v>
       </c>
       <c r="I18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1411,28 +1420,28 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F19">
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H19">
         <v>1</v>
       </c>
       <c r="I19" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J19" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1443,28 +1452,28 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H20">
         <v>2</v>
       </c>
       <c r="I20" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J20" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1475,28 +1484,28 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F21">
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H21">
         <v>3</v>
       </c>
       <c r="I21" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J21" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1507,28 +1516,28 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H22">
         <v>4</v>
       </c>
       <c r="I22" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J22" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1539,28 +1548,28 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F23">
         <v>2</v>
       </c>
       <c r="G23" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H23">
         <v>1</v>
       </c>
       <c r="I23" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J23" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1571,28 +1580,28 @@
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F24">
         <v>2</v>
       </c>
       <c r="G24" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H24">
         <v>2</v>
       </c>
       <c r="I24" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J24" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1603,28 +1612,28 @@
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F25">
         <v>3</v>
       </c>
       <c r="G25" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H25">
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J25" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1635,28 +1644,28 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D26">
         <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H26">
         <v>1</v>
       </c>
       <c r="I26" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J26" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1667,28 +1676,28 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D27">
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F27">
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H27">
         <v>2</v>
       </c>
       <c r="I27" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J27" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1699,28 +1708,28 @@
         <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D28">
         <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F28">
         <v>2</v>
       </c>
       <c r="G28" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H28">
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J28" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1731,28 +1740,28 @@
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D29">
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F29">
         <v>3</v>
       </c>
       <c r="G29" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H29">
         <v>1</v>
       </c>
       <c r="I29" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J29" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1763,28 +1772,28 @@
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D30">
         <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F30">
         <v>3</v>
       </c>
       <c r="G30" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H30">
         <v>2</v>
       </c>
       <c r="I30" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J30" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1795,28 +1804,28 @@
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D31">
         <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F31">
         <v>3</v>
       </c>
       <c r="G31" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H31">
         <v>3</v>
       </c>
       <c r="I31" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="J31" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1827,28 +1836,28 @@
         <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E32" t="s">
         <v>81</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G32" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H32">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I32" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="J32" t="s">
-        <v>127</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1859,10 +1868,10 @@
         <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E33" t="s">
         <v>82</v>
@@ -1871,16 +1880,16 @@
         <v>1</v>
       </c>
       <c r="G33" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H33">
         <v>1</v>
       </c>
       <c r="I33" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J33" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1891,28 +1900,28 @@
         <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D34">
         <v>4</v>
       </c>
       <c r="E34" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F34">
         <v>1</v>
       </c>
       <c r="G34" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I34" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="J34" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1923,28 +1932,28 @@
         <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D35">
         <v>4</v>
       </c>
       <c r="E35" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F35">
         <v>1</v>
       </c>
       <c r="G35" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H35">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I35" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="J35" t="s">
-        <v>96</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1955,25 +1964,28 @@
         <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D36">
         <v>4</v>
       </c>
       <c r="E36" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G36" t="s">
         <v>90</v>
       </c>
       <c r="H36">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I36" t="s">
-        <v>131</v>
+        <v>132</v>
+      </c>
+      <c r="J36" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -1981,19 +1993,19 @@
         <v>45</v>
       </c>
       <c r="B37">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C37" t="s">
         <v>77</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E37" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G37" t="s">
         <v>91</v>
@@ -2002,10 +2014,7 @@
         <v>1</v>
       </c>
       <c r="I37" t="s">
-        <v>132</v>
-      </c>
-      <c r="J37" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -2016,16 +2025,16 @@
         <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G38" t="s">
         <v>92</v>
@@ -2034,10 +2043,10 @@
         <v>1</v>
       </c>
       <c r="I38" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J38" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2048,28 +2057,28 @@
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F39">
         <v>2</v>
       </c>
       <c r="G39" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I39" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="J39" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -2080,28 +2089,28 @@
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F40">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G40" t="s">
         <v>93</v>
       </c>
       <c r="H40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I40" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="J40" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2112,16 +2121,16 @@
         <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F41">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G41" t="s">
         <v>94</v>
@@ -2130,10 +2139,10 @@
         <v>1</v>
       </c>
       <c r="I41" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="J41" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2144,28 +2153,28 @@
         <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E42" t="s">
         <v>80</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G42" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="H42">
         <v>1</v>
       </c>
       <c r="I42" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J42" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -2176,28 +2185,28 @@
         <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D43">
         <v>2</v>
       </c>
       <c r="E43" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G43" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H43">
         <v>1</v>
       </c>
       <c r="I43" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="J43" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -2208,28 +2217,28 @@
         <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D44">
         <v>2</v>
       </c>
       <c r="E44" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F44">
         <v>2</v>
       </c>
       <c r="G44" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I44" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J44" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2240,28 +2249,28 @@
         <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D45">
         <v>2</v>
       </c>
       <c r="E45" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G45" t="s">
         <v>88</v>
       </c>
       <c r="H45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I45" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J45" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2272,28 +2281,28 @@
         <v>5</v>
       </c>
       <c r="C46" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D46">
         <v>2</v>
       </c>
       <c r="E46" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F46">
         <v>3</v>
       </c>
       <c r="G46" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I46" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J46" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2304,28 +2313,28 @@
         <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D47">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E47" t="s">
         <v>81</v>
       </c>
       <c r="F47">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G47" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I47" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J47" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -2336,28 +2345,28 @@
         <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D48">
         <v>3</v>
       </c>
       <c r="E48" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F48">
         <v>1</v>
       </c>
       <c r="G48" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I48" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="J48" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2368,10 +2377,10 @@
         <v>5</v>
       </c>
       <c r="C49" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D49">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E49" t="s">
         <v>82</v>
@@ -2380,16 +2389,16 @@
         <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="H49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I49" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="J49" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2400,28 +2409,28 @@
         <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D50">
         <v>5</v>
       </c>
       <c r="E50" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G50" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I50" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J50" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2432,28 +2441,28 @@
         <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D51">
         <v>5</v>
       </c>
       <c r="E51" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F51">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G51" t="s">
         <v>96</v>
       </c>
       <c r="H51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I51" t="s">
-        <v>96</v>
+        <v>146</v>
       </c>
       <c r="J51" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2464,16 +2473,16 @@
         <v>5</v>
       </c>
       <c r="C52" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D52">
         <v>5</v>
       </c>
       <c r="E52" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F52">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G52" t="s">
         <v>97</v>
@@ -2482,10 +2491,10 @@
         <v>1</v>
       </c>
       <c r="I52" t="s">
-        <v>145</v>
+        <v>97</v>
       </c>
       <c r="J52" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2496,28 +2505,28 @@
         <v>5</v>
       </c>
       <c r="C53" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D53">
         <v>5</v>
       </c>
       <c r="E53" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F53">
         <v>4</v>
       </c>
       <c r="G53" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I53" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J53" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2528,28 +2537,28 @@
         <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D54">
         <v>5</v>
       </c>
       <c r="E54" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F54">
         <v>4</v>
       </c>
       <c r="G54" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H54">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I54" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J54" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2560,28 +2569,28 @@
         <v>5</v>
       </c>
       <c r="C55" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D55">
         <v>5</v>
       </c>
       <c r="E55" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F55">
         <v>4</v>
       </c>
       <c r="G55" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H55">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I55" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J55" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -2589,31 +2598,31 @@
         <v>64</v>
       </c>
       <c r="B56">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C56" t="s">
         <v>78</v>
       </c>
       <c r="D56">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E56" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F56">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G56" t="s">
         <v>98</v>
       </c>
       <c r="H56">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I56" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J56" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2624,28 +2633,28 @@
         <v>6</v>
       </c>
       <c r="C57" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D57">
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F57">
         <v>1</v>
       </c>
       <c r="G57" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I57" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="J57" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -2656,28 +2665,28 @@
         <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D58">
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G58" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="H58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I58" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="J58" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -2688,28 +2697,28 @@
         <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D59">
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F59">
         <v>2</v>
       </c>
       <c r="G59" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I59" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="J59" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -2720,28 +2729,28 @@
         <v>6</v>
       </c>
       <c r="C60" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D60">
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F60">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G60" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I60" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="J60" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -2752,28 +2761,28 @@
         <v>6</v>
       </c>
       <c r="C61" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E61" t="s">
         <v>80</v>
       </c>
       <c r="F61">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G61" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="H61">
         <v>1</v>
       </c>
       <c r="I61" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="J61" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -2784,28 +2793,28 @@
         <v>6</v>
       </c>
       <c r="C62" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D62">
         <v>2</v>
       </c>
       <c r="E62" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F62">
         <v>1</v>
       </c>
       <c r="G62" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I62" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="J62" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -2816,28 +2825,28 @@
         <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D63">
         <v>2</v>
       </c>
       <c r="E63" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F63">
         <v>1</v>
       </c>
       <c r="G63" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H63">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I63" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="J63" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -2848,25 +2857,57 @@
         <v>6</v>
       </c>
       <c r="C64" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D64">
+        <v>2</v>
+      </c>
+      <c r="E64" t="s">
+        <v>81</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+      <c r="G64" t="s">
+        <v>92</v>
+      </c>
+      <c r="H64">
         <v>3</v>
       </c>
-      <c r="E64" t="s">
-        <v>82</v>
-      </c>
-      <c r="F64">
-        <v>1</v>
-      </c>
-      <c r="H64">
-        <v>1</v>
-      </c>
       <c r="I64" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="J64" t="s">
-        <v>189</v>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B65">
+        <v>6</v>
+      </c>
+      <c r="C65" t="s">
+        <v>79</v>
+      </c>
+      <c r="D65">
+        <v>3</v>
+      </c>
+      <c r="E65" t="s">
+        <v>83</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="I65" t="s">
+        <v>158</v>
+      </c>
+      <c r="J65" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 2026: - Kalender pagina's planning en doorlopende taken verwijderd - Kalender 2026 toegevoegd - Matchingsdata geupdate - Mededelingen geupdate - Procesinformatie pagina wijzigingen en stroomschema verwijderd - Selectie pagina handmatig bij vrijwillige matching, groepsgewijs bij nederlands adres, registreren sunrisedatum, mededeling vorig jaar gematcht verwijderd
</commit_message>
<xml_diff>
--- a/topography.xlsx
+++ b/topography.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="172">
   <si>
     <t>section_order</t>
   </si>
@@ -52,9 +52,6 @@
     <t>265e3b99</t>
   </si>
   <si>
-    <t>Jf034</t>
-  </si>
-  <si>
     <t>QYZyv</t>
   </si>
   <si>
@@ -70,9 +67,6 @@
     <t>KaatD</t>
   </si>
   <si>
-    <t>jLIP5</t>
-  </si>
-  <si>
     <t>22b8f0e8</t>
   </si>
   <si>
@@ -91,12 +85,6 @@
     <t>3Ha14</t>
   </si>
   <si>
-    <t>SbweJ</t>
-  </si>
-  <si>
-    <t>8Qgw7</t>
-  </si>
-  <si>
     <t>7BIwg</t>
   </si>
   <si>
@@ -211,12 +199,6 @@
     <t>dba5494c</t>
   </si>
   <si>
-    <t>13DZ5</t>
-  </si>
-  <si>
-    <t>Wgpda</t>
-  </si>
-  <si>
     <t>GHyqP</t>
   </si>
   <si>
@@ -229,15 +211,9 @@
     <t>zDB6g</t>
   </si>
   <si>
-    <t>gEvxi</t>
-  </si>
-  <si>
     <t>fySE8</t>
   </si>
   <si>
-    <t>IDvHp</t>
-  </si>
-  <si>
     <t>Home</t>
   </si>
   <si>
@@ -313,15 +289,9 @@
     <t>Reanimatie</t>
   </si>
   <si>
-    <t>Processtart</t>
-  </si>
-  <si>
     <t>Changelog</t>
   </si>
   <si>
-    <t>Wijzigingen</t>
-  </si>
-  <si>
     <t>Procesopbouw</t>
   </si>
   <si>
@@ -337,9 +307,6 @@
     <t>Instellingen OSIRIS</t>
   </si>
   <si>
-    <t>Stroomschema</t>
-  </si>
-  <si>
     <t>Processtap</t>
   </si>
   <si>
@@ -355,12 +322,6 @@
     <t>Matchingsdata</t>
   </si>
   <si>
-    <t>Planning</t>
-  </si>
-  <si>
-    <t>Doorlopende taken</t>
-  </si>
-  <si>
     <t>Vrijwillige matching</t>
   </si>
   <si>
@@ -469,12 +430,6 @@
     <t>Reanimatie afgewezen, geen bezwaar gemaakt</t>
   </si>
   <si>
-    <t>Handmatig bij vrijwillige matching</t>
-  </si>
-  <si>
-    <t>Groepsgewijs bij Nederlands woonadres</t>
-  </si>
-  <si>
     <t>Versturen voor activiteit</t>
   </si>
   <si>
@@ -484,15 +439,9 @@
     <t>Registreren uitnodiging</t>
   </si>
   <si>
-    <t xml:space="preserve">Registreren sunrisedatum </t>
-  </si>
-  <si>
     <t>Selecteren groep uitgenodigd</t>
   </si>
   <si>
-    <t>Mededeling vorig jaar gematcht</t>
-  </si>
-  <si>
     <t>Herinnering invullen formulier voor activiteit</t>
   </si>
   <si>
@@ -568,12 +517,6 @@
     <t>M_REANIMEER_NOK</t>
   </si>
   <si>
-    <t>M-1-FOR-HANDM</t>
-  </si>
-  <si>
-    <t>M-1-FOR-WOON</t>
-  </si>
-  <si>
     <t>M-1-FOR-HER-ACT</t>
   </si>
   <si>
@@ -586,13 +529,7 @@
     <t>M-2-ACT-UIT</t>
   </si>
   <si>
-    <t>M-2-ACT-SUNRISE</t>
-  </si>
-  <si>
     <t>M-2-ACT-LIJST</t>
-  </si>
-  <si>
-    <t>M-3-OVE-VORIGJAARGEMATCHT</t>
   </si>
 </sst>
 </file>
@@ -950,7 +887,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J65"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -996,7 +933,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1008,7 +945,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1019,7 +956,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1031,7 +968,7 @@
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1042,7 +979,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1051,10 +988,13 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>101</v>
+        <v>92</v>
+      </c>
+      <c r="J4" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1065,7 +1005,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1074,13 +1014,13 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I5" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="J5" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1091,7 +1031,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1100,13 +1040,13 @@
         <v>1</v>
       </c>
       <c r="H6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I6" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="J6" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1117,7 +1057,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1126,13 +1066,13 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I7" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="J7" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1143,7 +1083,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1152,13 +1092,13 @@
         <v>1</v>
       </c>
       <c r="H8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I8" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J8" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1169,22 +1109,22 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>76</v>
       </c>
       <c r="H9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>106</v>
-      </c>
-      <c r="J9" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1195,22 +1135,22 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>76</v>
       </c>
       <c r="H10">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I10" t="s">
-        <v>107</v>
-      </c>
-      <c r="J10" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1221,7 +1161,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1230,13 +1170,13 @@
         <v>2</v>
       </c>
       <c r="G11" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I11" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1247,7 +1187,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1256,13 +1196,13 @@
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I12" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1270,25 +1210,22 @@
         <v>21</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="F13">
-        <v>2</v>
-      </c>
-      <c r="G13" t="s">
-        <v>84</v>
+        <v>1</v>
       </c>
       <c r="H13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>110</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1296,25 +1233,25 @@
         <v>22</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="F14">
-        <v>2</v>
-      </c>
-      <c r="G14" t="s">
-        <v>84</v>
+        <v>1</v>
       </c>
       <c r="H14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I14" t="s">
-        <v>111</v>
+        <v>101</v>
+      </c>
+      <c r="J14" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1322,22 +1259,31 @@
         <v>23</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
+      <c r="E15" t="s">
+        <v>72</v>
+      </c>
       <c r="F15">
         <v>1</v>
       </c>
+      <c r="G15" t="s">
+        <v>77</v>
+      </c>
       <c r="H15">
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>76</v>
+        <v>102</v>
+      </c>
+      <c r="J15" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1345,25 +1291,31 @@
         <v>24</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
+      <c r="E16" t="s">
+        <v>72</v>
+      </c>
       <c r="F16">
         <v>1</v>
       </c>
+      <c r="G16" t="s">
+        <v>77</v>
+      </c>
       <c r="H16">
         <v>2</v>
       </c>
       <c r="I16" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="J16" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1371,22 +1323,31 @@
         <v>25</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
+      <c r="E17" t="s">
+        <v>72</v>
+      </c>
       <c r="F17">
         <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>77</v>
       </c>
       <c r="H17">
         <v>3</v>
       </c>
       <c r="I17" t="s">
-        <v>113</v>
+        <v>104</v>
+      </c>
+      <c r="J17" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1394,22 +1355,31 @@
         <v>26</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
+      <c r="E18" t="s">
+        <v>72</v>
+      </c>
       <c r="F18">
         <v>1</v>
       </c>
+      <c r="G18" t="s">
+        <v>77</v>
+      </c>
       <c r="H18">
         <v>4</v>
       </c>
       <c r="I18" t="s">
-        <v>114</v>
+        <v>105</v>
+      </c>
+      <c r="J18" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1420,28 +1390,28 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G19" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="H19">
         <v>1</v>
       </c>
       <c r="I19" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="J19" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1452,28 +1422,28 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G20" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="H20">
         <v>2</v>
       </c>
       <c r="I20" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="J20" t="s">
-        <v>116</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1484,28 +1454,28 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G21" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I21" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="J21" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1516,28 +1486,28 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
         <v>77</v>
       </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
-        <v>80</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22" t="s">
-        <v>85</v>
-      </c>
       <c r="H22">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I22" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="J22" t="s">
-        <v>118</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1548,28 +1518,28 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
         <v>77</v>
       </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
-        <v>80</v>
-      </c>
-      <c r="F23">
-        <v>2</v>
-      </c>
-      <c r="G23" t="s">
-        <v>86</v>
-      </c>
       <c r="H23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I23" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="J23" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1580,28 +1550,28 @@
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E24" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24" t="s">
         <v>80</v>
       </c>
-      <c r="F24">
-        <v>2</v>
-      </c>
-      <c r="G24" t="s">
-        <v>86</v>
-      </c>
       <c r="H24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="J24" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1612,28 +1582,28 @@
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F25">
         <v>3</v>
       </c>
       <c r="G25" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="H25">
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="J25" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1644,28 +1614,28 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D26">
         <v>2</v>
       </c>
       <c r="E26" t="s">
+        <v>73</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26" t="s">
         <v>81</v>
       </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26" t="s">
-        <v>85</v>
-      </c>
       <c r="H26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I26" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="J26" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1676,28 +1646,28 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D27">
         <v>2</v>
       </c>
       <c r="E27" t="s">
+        <v>73</v>
+      </c>
+      <c r="F27">
+        <v>3</v>
+      </c>
+      <c r="G27" t="s">
         <v>81</v>
       </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27" t="s">
-        <v>85</v>
-      </c>
       <c r="H27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I27" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="J27" t="s">
-        <v>162</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1708,28 +1678,28 @@
         <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D28">
         <v>2</v>
       </c>
       <c r="E28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F28">
+        <v>3</v>
+      </c>
+      <c r="G28" t="s">
         <v>81</v>
       </c>
-      <c r="F28">
-        <v>2</v>
-      </c>
-      <c r="G28" t="s">
-        <v>88</v>
-      </c>
       <c r="H28">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I28" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="J28" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1740,28 +1710,28 @@
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F29">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="H29">
         <v>1</v>
       </c>
       <c r="I29" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="J29" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1772,28 +1742,28 @@
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E30" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F30">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G30" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="H30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I30" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="J30" t="s">
-        <v>164</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1804,28 +1774,28 @@
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D31">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E31" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F31">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G31" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="H31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I31" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="J31" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1836,28 +1806,28 @@
         <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D32">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E32" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32" t="s">
+        <v>82</v>
+      </c>
+      <c r="H32">
         <v>3</v>
       </c>
-      <c r="G32" t="s">
+      <c r="I32" t="s">
+        <v>119</v>
+      </c>
+      <c r="J32" t="s">
         <v>89</v>
-      </c>
-      <c r="H32">
-        <v>4</v>
-      </c>
-      <c r="I32" t="s">
-        <v>128</v>
-      </c>
-      <c r="J32" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1868,28 +1838,25 @@
         <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D33">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E33" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G33" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H33">
         <v>1</v>
       </c>
       <c r="I33" t="s">
-        <v>129</v>
-      </c>
-      <c r="J33" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1897,31 +1864,31 @@
         <v>42</v>
       </c>
       <c r="B34">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D34">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="F34">
         <v>1</v>
       </c>
       <c r="G34" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="H34">
         <v>1</v>
       </c>
       <c r="I34" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="J34" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1929,31 +1896,31 @@
         <v>43</v>
       </c>
       <c r="B35">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D35">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="F35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G35" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I35" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="J35" t="s">
-        <v>131</v>
+        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1961,31 +1928,31 @@
         <v>44</v>
       </c>
       <c r="B36">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D36">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="F36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G36" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I36" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="J36" t="s">
-        <v>97</v>
+        <v>151</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -1993,28 +1960,31 @@
         <v>45</v>
       </c>
       <c r="B37">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D37">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="F37">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G37" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="H37">
         <v>1</v>
       </c>
       <c r="I37" t="s">
-        <v>133</v>
+        <v>123</v>
+      </c>
+      <c r="J37" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -2025,28 +1995,28 @@
         <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F38">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G38" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="H38">
         <v>1</v>
       </c>
       <c r="I38" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="J38" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2057,28 +2027,28 @@
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E39" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G39" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="H39">
         <v>1</v>
       </c>
       <c r="I39" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="J39" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -2089,28 +2059,28 @@
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E40" t="s">
+        <v>73</v>
+      </c>
+      <c r="F40">
+        <v>2</v>
+      </c>
+      <c r="G40" t="s">
         <v>80</v>
       </c>
-      <c r="F40">
-        <v>2</v>
-      </c>
-      <c r="G40" t="s">
-        <v>93</v>
-      </c>
       <c r="H40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I40" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="J40" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2121,28 +2091,28 @@
         <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E41" t="s">
+        <v>73</v>
+      </c>
+      <c r="F41">
+        <v>2</v>
+      </c>
+      <c r="G41" t="s">
         <v>80</v>
       </c>
-      <c r="F41">
-        <v>3</v>
-      </c>
-      <c r="G41" t="s">
-        <v>94</v>
-      </c>
       <c r="H41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I41" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="J41" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2153,28 +2123,28 @@
         <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E42" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F42">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G42" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="H42">
         <v>1</v>
       </c>
       <c r="I42" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="J42" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -2185,28 +2155,28 @@
         <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D43">
         <v>2</v>
       </c>
       <c r="E43" t="s">
+        <v>73</v>
+      </c>
+      <c r="F43">
+        <v>3</v>
+      </c>
+      <c r="G43" t="s">
         <v>81</v>
       </c>
-      <c r="F43">
-        <v>1</v>
-      </c>
-      <c r="G43" t="s">
-        <v>85</v>
-      </c>
       <c r="H43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I43" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="J43" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -2217,28 +2187,28 @@
         <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D44">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E44" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G44" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="H44">
         <v>1</v>
       </c>
       <c r="I44" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="J44" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2249,28 +2219,28 @@
         <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D45">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E45" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G45" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="H45">
         <v>2</v>
       </c>
       <c r="I45" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="J45" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2281,28 +2251,28 @@
         <v>5</v>
       </c>
       <c r="C46" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D46">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E46" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F46">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H46">
         <v>1</v>
       </c>
       <c r="I46" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="J46" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2313,28 +2283,28 @@
         <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D47">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E47" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F47">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G47" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H47">
         <v>2</v>
       </c>
       <c r="I47" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="J47" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -2345,28 +2315,28 @@
         <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D48">
+        <v>5</v>
+      </c>
+      <c r="E48" t="s">
+        <v>75</v>
+      </c>
+      <c r="F48">
         <v>3</v>
       </c>
-      <c r="E48" t="s">
-        <v>82</v>
-      </c>
-      <c r="F48">
-        <v>1</v>
-      </c>
       <c r="G48" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H48">
         <v>1</v>
       </c>
       <c r="I48" t="s">
-        <v>143</v>
+        <v>89</v>
       </c>
       <c r="J48" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2377,28 +2347,28 @@
         <v>5</v>
       </c>
       <c r="C49" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D49">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E49" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F49">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G49" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I49" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="J49" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2409,28 +2379,28 @@
         <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D50">
         <v>5</v>
       </c>
       <c r="E50" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="F50">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G50" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I50" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="J50" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2441,28 +2411,28 @@
         <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D51">
         <v>5</v>
       </c>
       <c r="E51" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="F51">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G51" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H51">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I51" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="J51" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2473,28 +2443,28 @@
         <v>5</v>
       </c>
       <c r="C52" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D52">
         <v>5</v>
       </c>
       <c r="E52" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="F52">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G52" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="H52">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I52" t="s">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="J52" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2502,31 +2472,31 @@
         <v>61</v>
       </c>
       <c r="B53">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C53" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D53">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="F53">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G53" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="H53">
         <v>1</v>
       </c>
       <c r="I53" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="J53" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2534,31 +2504,31 @@
         <v>62</v>
       </c>
       <c r="B54">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C54" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D54">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="F54">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G54" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="H54">
         <v>2</v>
       </c>
       <c r="I54" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="J54" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2566,31 +2536,31 @@
         <v>63</v>
       </c>
       <c r="B55">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C55" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D55">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="F55">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G55" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="H55">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I55" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="J55" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -2598,31 +2568,31 @@
         <v>64</v>
       </c>
       <c r="B56">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C56" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D56">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E56" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F56">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G56" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="H56">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I56" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="J56" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2633,281 +2603,28 @@
         <v>6</v>
       </c>
       <c r="C57" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E57" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F57">
         <v>1</v>
       </c>
       <c r="G57" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="H57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I57" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="J57" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10">
-      <c r="A58" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B58">
-        <v>6</v>
-      </c>
-      <c r="C58" t="s">
-        <v>79</v>
-      </c>
-      <c r="D58">
-        <v>1</v>
-      </c>
-      <c r="E58" t="s">
-        <v>80</v>
-      </c>
-      <c r="F58">
-        <v>1</v>
-      </c>
-      <c r="G58" t="s">
-        <v>99</v>
-      </c>
-      <c r="H58">
-        <v>2</v>
-      </c>
-      <c r="I58" t="s">
-        <v>152</v>
-      </c>
-      <c r="J58" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10">
-      <c r="A59" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B59">
-        <v>6</v>
-      </c>
-      <c r="C59" t="s">
-        <v>79</v>
-      </c>
-      <c r="D59">
-        <v>1</v>
-      </c>
-      <c r="E59" t="s">
-        <v>80</v>
-      </c>
-      <c r="F59">
-        <v>2</v>
-      </c>
-      <c r="G59" t="s">
-        <v>93</v>
-      </c>
-      <c r="H59">
-        <v>1</v>
-      </c>
-      <c r="I59" t="s">
-        <v>153</v>
-      </c>
-      <c r="J59" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10">
-      <c r="A60" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B60">
-        <v>6</v>
-      </c>
-      <c r="C60" t="s">
-        <v>79</v>
-      </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-      <c r="E60" t="s">
-        <v>80</v>
-      </c>
-      <c r="F60">
-        <v>2</v>
-      </c>
-      <c r="G60" t="s">
-        <v>93</v>
-      </c>
-      <c r="H60">
-        <v>2</v>
-      </c>
-      <c r="I60" t="s">
-        <v>154</v>
-      </c>
-      <c r="J60" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10">
-      <c r="A61" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B61">
-        <v>6</v>
-      </c>
-      <c r="C61" t="s">
-        <v>79</v>
-      </c>
-      <c r="D61">
-        <v>1</v>
-      </c>
-      <c r="E61" t="s">
-        <v>80</v>
-      </c>
-      <c r="F61">
-        <v>3</v>
-      </c>
-      <c r="G61" t="s">
-        <v>95</v>
-      </c>
-      <c r="H61">
-        <v>1</v>
-      </c>
-      <c r="I61" t="s">
-        <v>137</v>
-      </c>
-      <c r="J61" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10">
-      <c r="A62" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B62">
-        <v>6</v>
-      </c>
-      <c r="C62" t="s">
-        <v>79</v>
-      </c>
-      <c r="D62">
-        <v>2</v>
-      </c>
-      <c r="E62" t="s">
-        <v>81</v>
-      </c>
-      <c r="F62">
-        <v>1</v>
-      </c>
-      <c r="G62" t="s">
-        <v>92</v>
-      </c>
-      <c r="H62">
-        <v>1</v>
-      </c>
-      <c r="I62" t="s">
-        <v>155</v>
-      </c>
-      <c r="J62" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10">
-      <c r="A63" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B63">
-        <v>6</v>
-      </c>
-      <c r="C63" t="s">
-        <v>79</v>
-      </c>
-      <c r="D63">
-        <v>2</v>
-      </c>
-      <c r="E63" t="s">
-        <v>81</v>
-      </c>
-      <c r="F63">
-        <v>1</v>
-      </c>
-      <c r="G63" t="s">
-        <v>92</v>
-      </c>
-      <c r="H63">
-        <v>2</v>
-      </c>
-      <c r="I63" t="s">
-        <v>156</v>
-      </c>
-      <c r="J63" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10">
-      <c r="A64" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B64">
-        <v>6</v>
-      </c>
-      <c r="C64" t="s">
-        <v>79</v>
-      </c>
-      <c r="D64">
-        <v>2</v>
-      </c>
-      <c r="E64" t="s">
-        <v>81</v>
-      </c>
-      <c r="F64">
-        <v>1</v>
-      </c>
-      <c r="G64" t="s">
-        <v>92</v>
-      </c>
-      <c r="H64">
-        <v>3</v>
-      </c>
-      <c r="I64" t="s">
-        <v>157</v>
-      </c>
-      <c r="J64" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10">
-      <c r="A65" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B65">
-        <v>6</v>
-      </c>
-      <c r="C65" t="s">
-        <v>79</v>
-      </c>
-      <c r="D65">
-        <v>3</v>
-      </c>
-      <c r="E65" t="s">
-        <v>83</v>
-      </c>
-      <c r="F65">
-        <v>1</v>
-      </c>
-      <c r="H65">
-        <v>1</v>
-      </c>
-      <c r="I65" t="s">
-        <v>158</v>
-      </c>
-      <c r="J65" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>